<commit_message>
Web Application for COT report
</commit_message>
<xml_diff>
--- a/data/Forexdata3.xlsx
+++ b/data/Forexdata3.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1449"/>
+  <dimension ref="A1:D1465"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26519,6 +26519,294 @@
         <v>71475</v>
       </c>
     </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>CANADIAN DOLLAR - CHICAGO MERCANTILE EXCHANGE</t>
+        </is>
+      </c>
+      <c r="B1450" t="inlineStr">
+        <is>
+          <t>11/21/2023</t>
+        </is>
+      </c>
+      <c r="C1450" t="n">
+        <v>19407</v>
+      </c>
+      <c r="D1450" t="n">
+        <v>84847</v>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>SWISS FRANC - CHICAGO MERCANTILE EXCHANGE</t>
+        </is>
+      </c>
+      <c r="B1451" t="inlineStr">
+        <is>
+          <t>11/21/2023</t>
+        </is>
+      </c>
+      <c r="C1451" t="n">
+        <v>4727</v>
+      </c>
+      <c r="D1451" t="n">
+        <v>23721</v>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>BRITISH POUND STERLING - CHICAGO MERCANTILE EXCHANGE</t>
+        </is>
+      </c>
+      <c r="B1452" t="inlineStr">
+        <is>
+          <t>11/21/2023</t>
+        </is>
+      </c>
+      <c r="C1452" t="n">
+        <v>43300</v>
+      </c>
+      <c r="D1452" t="n">
+        <v>69398</v>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>JAPANESE YEN - CHICAGO MERCANTILE EXCHANGE</t>
+        </is>
+      </c>
+      <c r="B1453" t="inlineStr">
+        <is>
+          <t>11/21/2023</t>
+        </is>
+      </c>
+      <c r="C1453" t="n">
+        <v>39236</v>
+      </c>
+      <c r="D1453" t="n">
+        <v>144690</v>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>U.S. DOLLAR INDEX - ICE FUTURES U.S.</t>
+        </is>
+      </c>
+      <c r="B1454" t="inlineStr">
+        <is>
+          <t>11/21/2023</t>
+        </is>
+      </c>
+      <c r="C1454" t="n">
+        <v>28543</v>
+      </c>
+      <c r="D1454" t="n">
+        <v>7846</v>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>EURO FX - CHICAGO MERCANTILE EXCHANGE</t>
+        </is>
+      </c>
+      <c r="B1455" t="inlineStr">
+        <is>
+          <t>11/21/2023</t>
+        </is>
+      </c>
+      <c r="C1455" t="n">
+        <v>231095</v>
+      </c>
+      <c r="D1455" t="n">
+        <v>101441</v>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>NEW ZEALAND DOLLAR - CHICAGO MERCANTILE EXCHANGE</t>
+        </is>
+      </c>
+      <c r="B1456" t="inlineStr">
+        <is>
+          <t>11/21/2023</t>
+        </is>
+      </c>
+      <c r="C1456" t="n">
+        <v>7958</v>
+      </c>
+      <c r="D1456" t="n">
+        <v>24812</v>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>AUSTRALIAN DOLLAR - CHICAGO MERCANTILE EXCHANGE</t>
+        </is>
+      </c>
+      <c r="B1457" t="inlineStr">
+        <is>
+          <t>11/21/2023</t>
+        </is>
+      </c>
+      <c r="C1457" t="n">
+        <v>29565</v>
+      </c>
+      <c r="D1457" t="n">
+        <v>107535</v>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>CANADIAN DOLLAR - CHICAGO MERCANTILE EXCHANGE</t>
+        </is>
+      </c>
+      <c r="B1458" t="inlineStr">
+        <is>
+          <t>11/28/2023</t>
+        </is>
+      </c>
+      <c r="C1458" t="n">
+        <v>18991</v>
+      </c>
+      <c r="D1458" t="n">
+        <v>82233</v>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>SWISS FRANC - CHICAGO MERCANTILE EXCHANGE</t>
+        </is>
+      </c>
+      <c r="B1459" t="inlineStr">
+        <is>
+          <t>11/28/2023</t>
+        </is>
+      </c>
+      <c r="C1459" t="n">
+        <v>4300</v>
+      </c>
+      <c r="D1459" t="n">
+        <v>24589</v>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>BRITISH POUND STERLING - CHICAGO MERCANTILE EXCHANGE</t>
+        </is>
+      </c>
+      <c r="B1460" t="inlineStr">
+        <is>
+          <t>11/28/2023</t>
+        </is>
+      </c>
+      <c r="C1460" t="n">
+        <v>61296</v>
+      </c>
+      <c r="D1460" t="n">
+        <v>69191</v>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>JAPANESE YEN - CHICAGO MERCANTILE EXCHANGE</t>
+        </is>
+      </c>
+      <c r="B1461" t="inlineStr">
+        <is>
+          <t>11/28/2023</t>
+        </is>
+      </c>
+      <c r="C1461" t="n">
+        <v>30461</v>
+      </c>
+      <c r="D1461" t="n">
+        <v>139698</v>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>U.S. DOLLAR INDEX - ICE FUTURES U.S.</t>
+        </is>
+      </c>
+      <c r="B1462" t="inlineStr">
+        <is>
+          <t>11/28/2023</t>
+        </is>
+      </c>
+      <c r="C1462" t="n">
+        <v>28798</v>
+      </c>
+      <c r="D1462" t="n">
+        <v>9711</v>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>EURO FX - CHICAGO MERCANTILE EXCHANGE</t>
+        </is>
+      </c>
+      <c r="B1463" t="inlineStr">
+        <is>
+          <t>11/28/2023</t>
+        </is>
+      </c>
+      <c r="C1463" t="n">
+        <v>233454</v>
+      </c>
+      <c r="D1463" t="n">
+        <v>90289</v>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>NEW ZEALAND DOLLAR - CHICAGO MERCANTILE EXCHANGE</t>
+        </is>
+      </c>
+      <c r="B1464" t="inlineStr">
+        <is>
+          <t>11/28/2023</t>
+        </is>
+      </c>
+      <c r="C1464" t="n">
+        <v>10104</v>
+      </c>
+      <c r="D1464" t="n">
+        <v>29713</v>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>AUSTRALIAN DOLLAR - CHICAGO MERCANTILE EXCHANGE</t>
+        </is>
+      </c>
+      <c r="B1465" t="inlineStr">
+        <is>
+          <t>11/28/2023</t>
+        </is>
+      </c>
+      <c r="C1465" t="n">
+        <v>29203</v>
+      </c>
+      <c r="D1465" t="n">
+        <v>100422</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>